<commit_message>
nuevo intento de despliegue por render
</commit_message>
<xml_diff>
--- a/app/Plantillas.json/Entrada/eje2.xlsx
+++ b/app/Plantillas.json/Entrada/eje2.xlsx
@@ -769,15 +769,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE238D1-79D9-4780-82A4-2E88CD365F27}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{286B9658-108F-478C-9DB7-061A5BC50B5F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65A4A029-58B8-4A8A-89B4-97F1DB7AC524}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B8F09CC-7ACB-442C-BA36-C4A6D2C5A097}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24D3D85-EAFD-48BC-9744-AA99F8287233}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05EB8EA1-0A83-4D8F-9308-9BA852B39E9A}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>